<commit_message>
Got rid of user, shared workbook, fixed the items
</commit_message>
<xml_diff>
--- a/LostAndFound/LostAndFound/Resources/Disposal.xlsx
+++ b/LostAndFound/LostAndFound/Resources/Disposal.xlsx
@@ -15,6 +15,9 @@
     <sheet name="Disposed" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <customWorkbookViews>
+    <customWorkbookView name="Carlee Brady - Personal View" guid="{6664D292-16DD-455F-A0BE-B3277E91492A}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
+  </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="86">
   <si>
     <t>ItemDescription</t>
   </si>
@@ -276,6 +279,12 @@
   </si>
   <si>
     <t>libray</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>Email</t>
   </si>
 </sst>
 </file>
@@ -345,6 +354,24 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{1BE51AB3-8E7C-443A-B948-7E237DC102D3}">
+  <header guid="{1BE51AB3-8E7C-443A-B948-7E237DC102D3}" dateTime="2015-04-16T16:44:09" maxSheetId="2" userName="Carlee Brady" r:id="rId1">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+</headers>
+</file>
+
+<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
+</file>
+
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -610,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,11 +650,12 @@
     <col min="3" max="3" width="86" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="22.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>78</v>
       </c>
@@ -643,14 +671,20 @@
       <c r="E1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>42087</v>
       </c>
@@ -663,14 +697,14 @@
       <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>42058</v>
       </c>
@@ -683,11 +717,11 @@
       <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>42058</v>
       </c>
@@ -700,11 +734,11 @@
       <c r="D4" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>42058</v>
       </c>
@@ -717,11 +751,11 @@
       <c r="D5" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>42058</v>
       </c>
@@ -734,11 +768,11 @@
       <c r="D6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>42024</v>
       </c>
@@ -754,14 +788,14 @@
       <c r="E7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I7" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>42038</v>
       </c>
@@ -777,14 +811,14 @@
       <c r="E8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I8" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>42053</v>
       </c>
@@ -797,14 +831,14 @@
       <c r="E9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I9" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>42048</v>
       </c>
@@ -820,14 +854,14 @@
       <c r="E10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I10" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>42083</v>
       </c>
@@ -843,14 +877,14 @@
       <c r="E11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I11" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>42083</v>
       </c>
@@ -860,14 +894,14 @@
       <c r="E12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I12" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>42080</v>
       </c>
@@ -883,14 +917,14 @@
       <c r="E13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I13" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>42093</v>
       </c>
@@ -906,14 +940,14 @@
       <c r="E14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I14" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>42012</v>
       </c>
@@ -929,14 +963,14 @@
       <c r="E15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I15" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>41960</v>
       </c>
@@ -952,14 +986,14 @@
       <c r="E16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="H16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I16" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>42058</v>
       </c>
@@ -972,11 +1006,11 @@
       <c r="D17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="I17" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>42058</v>
       </c>
@@ -989,11 +1023,11 @@
       <c r="D18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="I18" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>42058</v>
       </c>
@@ -1006,11 +1040,11 @@
       <c r="D19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="I19" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>42053</v>
       </c>
@@ -1023,14 +1057,14 @@
       <c r="E20" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="H20" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I20" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>42058</v>
       </c>
@@ -1043,11 +1077,11 @@
       <c r="D21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="I21" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>42033</v>
       </c>
@@ -1060,14 +1094,14 @@
       <c r="E22" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I22" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>42038</v>
       </c>
@@ -1080,14 +1114,14 @@
       <c r="E23" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="H23" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I23" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>42044</v>
       </c>
@@ -1100,14 +1134,14 @@
       <c r="E24" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="H24" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G24" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I24" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>42089</v>
       </c>
@@ -1120,11 +1154,11 @@
       <c r="D25" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="I25" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>42044</v>
       </c>
@@ -1137,14 +1171,14 @@
       <c r="E26" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="H26" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G26" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I26" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>42058</v>
       </c>
@@ -1157,11 +1191,11 @@
       <c r="D27" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="I27" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>42058</v>
       </c>
@@ -1174,11 +1208,11 @@
       <c r="D28" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="I28" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>42089</v>
       </c>
@@ -1191,11 +1225,11 @@
       <c r="D29" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="I29" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>42089</v>
       </c>
@@ -1208,11 +1242,11 @@
       <c r="D30" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G30" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I30" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>42089</v>
       </c>
@@ -1225,11 +1259,11 @@
       <c r="D31" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G31" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I31" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>42089</v>
       </c>
@@ -1242,11 +1276,11 @@
       <c r="D32" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G32" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I32" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>42089</v>
       </c>
@@ -1259,11 +1293,11 @@
       <c r="D33" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G33" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I33" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>42089</v>
       </c>
@@ -1276,11 +1310,11 @@
       <c r="D34" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G34" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I34" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>42081</v>
       </c>
@@ -1293,14 +1327,14 @@
       <c r="E35" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="H35" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G35" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I35" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>42058</v>
       </c>
@@ -1313,11 +1347,11 @@
       <c r="D36" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="I36" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>42060</v>
       </c>
@@ -1330,11 +1364,11 @@
       <c r="D37" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="I37" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>42060</v>
       </c>
@@ -1347,11 +1381,11 @@
       <c r="D38" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="I38" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>42060</v>
       </c>
@@ -1364,11 +1398,11 @@
       <c r="D39" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="I39" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>42058</v>
       </c>
@@ -1381,11 +1415,11 @@
       <c r="D40" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G40" s="2" t="s">
+      <c r="I40" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>42089</v>
       </c>
@@ -1395,11 +1429,11 @@
       <c r="C41" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="I41" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>42058</v>
       </c>
@@ -1412,11 +1446,11 @@
       <c r="D42" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="I42" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42089</v>
       </c>
@@ -1429,11 +1463,11 @@
       <c r="D43" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="I43" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42089</v>
       </c>
@@ -1446,11 +1480,11 @@
       <c r="D44" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="I44" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>42080</v>
       </c>
@@ -1466,14 +1500,14 @@
       <c r="E45" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="H45" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G45" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I45" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>42089</v>
       </c>
@@ -1483,16 +1517,22 @@
       <c r="C46" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G46" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G47" s="2" t="s">
+      <c r="I46" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I47" s="2" t="s">
         <v>81</v>
       </c>
     </row>
   </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{6664D292-16DD-455F-A0BE-B3277E91492A}" topLeftCell="D1">
+      <selection activeCell="G1" sqref="G1"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+  </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>